<commit_message>
Added Global Profiling Gliders
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GP05MOAS-PG515_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GP05MOAS-PG515_00001.xlsx
@@ -5,35 +5,35 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\IRAD\IRAD 2015\Programs\OOI Phase 2\Post Delivery 7 support\Asset Management Data\ingestion-csvs_20151204\ingestion-csvs\GP05MOAS-PG515\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="60" yWindow="7980" windowWidth="25032" windowHeight="11580" tabRatio="377" activeTab="1"/>
+    <workbookView xWindow="60" yWindow="7980" windowWidth="25035" windowHeight="11580" tabRatio="377" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
     <sheet name="Asset_Cal_Info" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Asset_Cal_Info!$A$1:$H$19</definedName>
-    <definedName name="_xlnm._FilterDatabase">Asset_Cal_Info!$A$1:$H$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Asset_Cal_Info!$A$1:$H$15</definedName>
+    <definedName name="_xlnm._FilterDatabase">Asset_Cal_Info!$A$1:$H$15</definedName>
     <definedName name="_FilterDatabase_0">Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0">Moorings!$B$1:$K$79</definedName>
     <definedName name="_FilterDatabase_0_0_0">Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0_0">Moorings!$B$1:$K$79</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0">Asset_Cal_Info!$A$1:$H$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0">Asset_Cal_Info!$A$1:$H$386</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0">Asset_Cal_Info!$A$1:$H$387</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0_0_0">Asset_Cal_Info!$A$1:$H$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0">Asset_Cal_Info!$A$1:$H$386</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_1">Asset_Cal_Info!$A$1:$H$386</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0">Asset_Cal_Info!$A$1:$H$387</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_1">Asset_Cal_Info!$A$1:$H$387</definedName>
     <definedName name="_FilterDatabase_0_0_0_1">Asset_Cal_Info!$A$1:$H$1</definedName>
-    <definedName name="_FilterDatabase_0_0_1">Asset_Cal_Info!$A$1:$H$386</definedName>
+    <definedName name="_FilterDatabase_0_0_1">Asset_Cal_Info!$A$1:$H$387</definedName>
     <definedName name="_FilterDatabase_0_1">Asset_Cal_Info!$A$1:$H$1</definedName>
-    <definedName name="_FilterDatabase_1">Asset_Cal_Info!$A$1:$H$19</definedName>
+    <definedName name="_FilterDatabase_1">Asset_Cal_Info!$A$1:$H$15</definedName>
     <definedName name="_FilterDatabase_1_1">Asset_Cal_Info!$A$1:$H$1</definedName>
     <definedName name="_FilterDatabase_1_1_1">Moorings!$B$1:$K$79</definedName>
-    <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$H$386</definedName>
+    <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$H$387</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="46">
   <si>
     <t>Ref Des</t>
   </si>
@@ -113,15 +113,6 @@
     <t>GP05MOAS-PG515-01-CTDGVM000</t>
   </si>
   <si>
-    <t>GP05MOAS-PG515-02-FLORTM000</t>
-  </si>
-  <si>
-    <t>GP05MOAS-PG515-03-FLORTO000</t>
-  </si>
-  <si>
-    <t>GP05MOAS-PG515-04-PARADM000</t>
-  </si>
-  <si>
     <t>GP05MOAS-PG515-00-ENG000000</t>
   </si>
   <si>
@@ -140,15 +131,6 @@
     <t>CC_scattering_angle</t>
   </si>
   <si>
-    <t>CC_2_measurement_wavelength</t>
-  </si>
-  <si>
-    <t>CC_3_measurement_wavelength</t>
-  </si>
-  <si>
-    <t>CC_1_measurement_wavelength</t>
-  </si>
-  <si>
     <t>Mooring OOIBARCODE</t>
   </si>
   <si>
@@ -165,6 +147,42 @@
   </si>
   <si>
     <t>A01223</t>
+  </si>
+  <si>
+    <t>GP05MOAS-PG515-03-FLORTM000</t>
+  </si>
+  <si>
+    <t>GP05MOAS-PG515-04-FLORTO000</t>
+  </si>
+  <si>
+    <t>GP05MOAS-PG515-06-PARADM000</t>
+  </si>
+  <si>
+    <t>GP05MOAS-PG515-02-DOSTAM000</t>
+  </si>
+  <si>
+    <t>GP05MOAS-PG515-05-NUTNRM000</t>
+  </si>
+  <si>
+    <t>CC_wl</t>
+  </si>
+  <si>
+    <t>CC_cal_temp</t>
+  </si>
+  <si>
+    <t>CC_eno3</t>
+  </si>
+  <si>
+    <t>CC_eswa</t>
+  </si>
+  <si>
+    <t>CC_di</t>
+  </si>
+  <si>
+    <t>CC_lower_wavelength_limit_for_spectra_fit</t>
+  </si>
+  <si>
+    <t>CC_upper_wavelength_limit_for_spectra_fit</t>
   </si>
 </sst>
 </file>
@@ -174,7 +192,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -284,8 +302,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -301,12 +325,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -384,7 +402,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -442,7 +460,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -462,10 +479,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="11" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -478,6 +491,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="Excel Built-in Normal" xfId="14"/>
@@ -876,59 +890,59 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" customWidth="1"/>
-    <col min="2" max="2" width="31.44140625" customWidth="1"/>
-    <col min="3" max="4" width="15.88671875" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" customWidth="1"/>
+    <col min="3" max="4" width="15.85546875" customWidth="1"/>
     <col min="5" max="9" width="19" customWidth="1"/>
-    <col min="10" max="11" width="13.109375" customWidth="1"/>
-    <col min="12" max="12" width="29.109375" customWidth="1"/>
-    <col min="13" max="13" width="17.88671875" customWidth="1"/>
-    <col min="14" max="14" width="18.33203125" customWidth="1"/>
+    <col min="10" max="11" width="13.140625" customWidth="1"/>
+    <col min="12" max="12" width="29.140625" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" customWidth="1"/>
+    <col min="14" max="14" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="36" t="s">
+    <row r="1" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="33" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>20</v>
@@ -970,7 +984,7 @@
         <v>-144.5446</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
@@ -987,57 +1001,57 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" customWidth="1"/>
+    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" customWidth="1"/>
-    <col min="7" max="7" width="22" customWidth="1"/>
-    <col min="8" max="8" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="37" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:17" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="35" t="s">
+      <c r="B1" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="35" t="s">
+      <c r="E1" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="H1" s="32" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C2" s="16">
         <v>515</v>
@@ -1046,7 +1060,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F2" s="14">
         <v>9231</v>
@@ -1062,7 +1076,7 @@
       <c r="M2" s="10"/>
       <c r="N2" s="10"/>
     </row>
-    <row r="3" spans="1:17" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="16"/>
@@ -1078,12 +1092,12 @@
       <c r="M3" s="10"/>
       <c r="N3" s="10"/>
     </row>
-    <row r="4" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
-        <v>22</v>
+    <row r="4" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C4" s="16">
         <v>515</v>
@@ -1092,136 +1106,131 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F4" s="21">
         <v>3501</v>
       </c>
-      <c r="G4" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="33">
+      <c r="G4" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="30">
         <v>124</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
     </row>
-    <row r="5" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="23" t="s">
-        <v>22</v>
+    <row r="5" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="24">
+        <v>33</v>
+      </c>
+      <c r="C5" s="23">
         <v>515</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="24">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="26">
+        <v>31</v>
+      </c>
+      <c r="F5" s="25">
         <v>3501</v>
       </c>
-      <c r="G5" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="28">
+      <c r="G5" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="27">
         <v>700</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5" s="29"/>
+        <v>24</v>
+      </c>
+      <c r="J5" s="28"/>
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
     </row>
-    <row r="6" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
-        <v>22</v>
+    <row r="6" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="24">
+        <v>33</v>
+      </c>
+      <c r="C6" s="23">
         <v>515</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="24">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="26">
+        <v>31</v>
+      </c>
+      <c r="F6" s="25">
         <v>3501</v>
       </c>
-      <c r="G6" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="34">
+      <c r="G6" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="31">
         <v>1.0760000000000001</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" s="29"/>
+        <v>24</v>
+      </c>
+      <c r="J6" s="28"/>
       <c r="K6" s="10"/>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
     </row>
-    <row r="7" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="23" t="s">
-        <v>22</v>
+    <row r="7" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="24">
+        <v>33</v>
+      </c>
+      <c r="C7" s="23">
         <v>515</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="24">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="26">
+        <v>31</v>
+      </c>
+      <c r="F7" s="25">
         <v>3501</v>
       </c>
-      <c r="G7" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="30">
+      <c r="G7" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="29">
         <v>3.9E-2</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="J7" s="29"/>
+        <v>24</v>
+      </c>
+      <c r="J7" s="28"/>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
     </row>
-    <row r="8" spans="1:17" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="19"/>
       <c r="B8" s="19"/>
       <c r="C8" s="20"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="11"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
@@ -1229,148 +1238,159 @@
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
     </row>
-    <row r="9" spans="1:17" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="I9" s="19" t="s">
+    <row r="9" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="16">
+        <v>515</v>
+      </c>
+      <c r="D9" s="24">
+        <v>1</v>
+      </c>
+      <c r="F9" s="24">
+        <v>1239</v>
+      </c>
+      <c r="G9" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="16">
+      <c r="H9" s="27">
+        <v>700</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="P9" s="10"/>
+    </row>
+    <row r="10" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="16">
         <v>515</v>
       </c>
-      <c r="K9" s="12">
+      <c r="D10" s="24">
         <v>1</v>
       </c>
-      <c r="L9" s="12">
+      <c r="F10" s="24">
         <v>1239</v>
       </c>
-      <c r="M9" s="31" t="s">
+      <c r="G10" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="30">
+        <v>124</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="10"/>
+    </row>
+    <row r="11" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="N9" s="32">
-        <v>650</v>
-      </c>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-    </row>
-    <row r="10" spans="1:17" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="I10" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" s="24">
+      <c r="C11" s="16">
         <v>515</v>
       </c>
-      <c r="K10" s="25">
+      <c r="D11" s="24">
         <v>1</v>
       </c>
-      <c r="L10" s="25">
+      <c r="F11" s="24">
         <v>1239</v>
       </c>
-      <c r="M10" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="N10" s="32">
-        <v>532</v>
-      </c>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-    </row>
-    <row r="11" spans="1:17" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="I11" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="J11" s="24">
+      <c r="G11" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="31">
+        <v>1.0760000000000001</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="P11" s="28"/>
+      <c r="Q11" s="10"/>
+    </row>
+    <row r="12" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="16">
         <v>515</v>
       </c>
-      <c r="K11" s="25">
+      <c r="D12" s="24">
         <v>1</v>
       </c>
-      <c r="L11" s="25">
+      <c r="F12" s="24">
         <v>1239</v>
       </c>
-      <c r="M11" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="N11" s="32">
-        <v>470</v>
-      </c>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-    </row>
-    <row r="12" spans="1:17" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="I12" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="J12" s="24">
+      <c r="G12" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="29">
+        <v>3.9E-2</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="P12" s="28"/>
+      <c r="Q12" s="10"/>
+    </row>
+    <row r="13" spans="1:17" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+    </row>
+    <row r="14" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="16">
         <v>515</v>
       </c>
-      <c r="K12" s="25">
+      <c r="D14" s="12">
         <v>1</v>
       </c>
-      <c r="L12" s="25">
-        <v>1239</v>
-      </c>
-      <c r="M12" s="27" t="s">
+      <c r="E14" t="s">
         <v>30</v>
       </c>
-      <c r="N12" s="33">
-        <v>124</v>
-      </c>
-      <c r="O12" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="10"/>
-    </row>
-    <row r="13" spans="1:17" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="I13" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="J13" s="24">
-        <v>515</v>
-      </c>
-      <c r="K13" s="25">
-        <v>1</v>
-      </c>
-      <c r="L13" s="25">
-        <v>1239</v>
-      </c>
-      <c r="M13" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="N13" s="34">
-        <v>1.0760000000000001</v>
-      </c>
-      <c r="O13" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="10"/>
-    </row>
-    <row r="14" spans="1:17" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="I14" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="J14" s="24">
-        <v>515</v>
-      </c>
-      <c r="K14" s="25">
-        <v>1</v>
-      </c>
-      <c r="L14" s="25">
-        <v>1239</v>
-      </c>
-      <c r="M14" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="N14" s="30">
-        <v>3.9E-2</v>
-      </c>
-      <c r="O14" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="10"/>
-    </row>
-    <row r="15" spans="1:17" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="F14" s="12">
+        <v>50185</v>
+      </c>
+      <c r="G14" s="13"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="16"/>
@@ -1386,12 +1406,12 @@
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
     </row>
-    <row r="16" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="9" t="s">
-        <v>24</v>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C16" s="16">
         <v>515</v>
@@ -1399,40 +1419,16 @@
       <c r="D16" s="12">
         <v>1</v>
       </c>
-      <c r="E16" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" s="12">
-        <v>50185</v>
-      </c>
-      <c r="G16" s="13"/>
-      <c r="H16" s="18"/>
       <c r="I16" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-    </row>
-    <row r="18" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
-        <v>25</v>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C18" s="16">
         <v>515</v>
@@ -1440,40 +1436,95 @@
       <c r="D18" s="12">
         <v>1</v>
       </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="14">
+      <c r="G18" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I18" s="10"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C19" s="16"/>
+      <c r="D19" s="12"/>
+      <c r="G19" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="I19" s="10"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C20" s="16"/>
+      <c r="D20" s="12"/>
+      <c r="G20" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="I20" s="10"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C21" s="16"/>
+      <c r="D21" s="12"/>
+      <c r="G21" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="I21" s="10"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C22" s="16"/>
+      <c r="D22" s="12"/>
+      <c r="G22" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="I22" s="10"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C23" s="16"/>
+      <c r="D23" s="12"/>
+      <c r="G23" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="I23" s="10"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C24" s="16"/>
+      <c r="D24" s="12"/>
+      <c r="G24" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="I24" s="10"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C25" s="16"/>
+      <c r="D25" s="12"/>
+      <c r="I25" s="10"/>
+    </row>
+    <row r="26" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="16">
         <v>515</v>
       </c>
-      <c r="G18" s="10"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="10" t="s">
+      <c r="D26" s="12">
+        <v>1</v>
+      </c>
+      <c r="E26" s="12"/>
+      <c r="F26" s="14">
+        <v>515</v>
+      </c>
+      <c r="G26" s="10"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-    </row>
-    <row r="19" spans="1:14" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>